<commit_message>
tambah field rt rw di Nama-nama Perusahaan.xlsx
</commit_message>
<xml_diff>
--- a/DOKUMEN  PENDUKUNG/DATA DATA YANG HARUS DIMASUKAN/EKONOMI/Nama-nama Perusahaan.xlsx
+++ b/DOKUMEN  PENDUKUNG/DATA DATA YANG HARUS DIMASUKAN/EKONOMI/Nama-nama Perusahaan.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sipepeng\DOKUMEN  PENDUKUNG\DATA DATA YANG HARUS DIMASUKAN\EKONOMI\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="15120" windowHeight="8010"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="101">
   <si>
     <t>NO</t>
   </si>
@@ -292,13 +297,40 @@
   </si>
   <si>
     <t>Angkutan (Container)</t>
+  </si>
+  <si>
+    <t>RT</t>
+  </si>
+  <si>
+    <t>RW</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>09</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -359,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -397,6 +429,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -404,6 +451,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -450,7 +505,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -482,9 +537,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -516,6 +572,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -691,14 +748,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="2" width="32.42578125" customWidth="1"/>
@@ -709,7 +766,7 @@
     <col min="7" max="7" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>82</v>
       </c>
@@ -720,7 +777,7 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>83</v>
       </c>
@@ -731,7 +788,7 @@
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="33" customHeight="1">
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
@@ -753,8 +810,14 @@
       <c r="G4" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1">
+      <c r="H4" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>1</v>
       </c>
@@ -776,8 +839,10 @@
       <c r="G5" s="6">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="17.25" customHeight="1">
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+    </row>
+    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -799,8 +864,14 @@
       <c r="G6" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="17.25" customHeight="1">
+      <c r="H6" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -822,8 +893,14 @@
       <c r="G7" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="17.25" customHeight="1">
+      <c r="H7" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -845,8 +922,14 @@
       <c r="G8" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="17.25" customHeight="1">
+      <c r="H8" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>4</v>
       </c>
@@ -868,8 +951,14 @@
       <c r="G9" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="17.25" customHeight="1">
+      <c r="H9" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>5</v>
       </c>
@@ -891,8 +980,14 @@
       <c r="G10" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="17.25" customHeight="1">
+      <c r="H10" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>6</v>
       </c>
@@ -914,8 +1009,14 @@
       <c r="G11" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="17.25" customHeight="1">
+      <c r="H11" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="I11" s="18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>7</v>
       </c>
@@ -937,8 +1038,14 @@
       <c r="G12" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="17.25" customHeight="1">
+      <c r="H12" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>8</v>
       </c>
@@ -960,8 +1067,14 @@
       <c r="G13" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="17.25" customHeight="1">
+      <c r="H13" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>9</v>
       </c>
@@ -983,8 +1096,14 @@
       <c r="G14" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="17.25" customHeight="1">
+      <c r="H14" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>10</v>
       </c>
@@ -1006,8 +1125,14 @@
       <c r="G15" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="17.25" customHeight="1">
+      <c r="H15" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="I15" s="18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>11</v>
       </c>
@@ -1029,8 +1154,14 @@
       <c r="G16" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="19.5" customHeight="1">
+      <c r="H16" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>12</v>
       </c>
@@ -1052,8 +1183,14 @@
       <c r="G17" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="28.5" customHeight="1">
+      <c r="H17" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>13</v>
       </c>
@@ -1075,8 +1212,14 @@
       <c r="G18" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="17.25" customHeight="1">
+      <c r="H18" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>14</v>
       </c>
@@ -1098,8 +1241,14 @@
       <c r="G19" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="17.25" customHeight="1">
+      <c r="H19" s="18">
+        <v>74</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>15</v>
       </c>
@@ -1121,8 +1270,14 @@
       <c r="G20" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="17.25" customHeight="1">
+      <c r="H20" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>16</v>
       </c>
@@ -1144,8 +1299,14 @@
       <c r="G21" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="17.25" customHeight="1">
+      <c r="H21" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>17</v>
       </c>
@@ -1167,8 +1328,14 @@
       <c r="G22" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="17.25" customHeight="1">
+      <c r="H22" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="I22" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>18</v>
       </c>
@@ -1190,8 +1357,14 @@
       <c r="G23" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="17.25" customHeight="1">
+      <c r="H23" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="I23" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>19</v>
       </c>
@@ -1211,14 +1384,20 @@
       <c r="G24" s="3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="15" customHeight="1">
+      <c r="H24" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="I24" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F26" s="13" t="s">
         <v>90</v>
       </c>
       <c r="G26" s="13"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E27" s="9" t="s">
         <v>86</v>
       </c>
@@ -1227,17 +1406,17 @@
       </c>
       <c r="G27" s="12"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F32" s="10" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="6:6">
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
         <v>89</v>
       </c>
@@ -1255,24 +1434,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>